<commit_message>
Set up to try output nest
</commit_message>
<xml_diff>
--- a/test/MPSGEresults.xlsx
+++ b/test/MPSGEresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\.julia\dev\MPSGE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B019F-EE8C-498E-A4B2-0F1C4FF83561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05A2C7E-FB3F-4F75-BDDC-59E3BA4DEEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="9072" firstSheet="5" activeTab="5" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9072" firstSheet="7" activeTab="9" xr2:uid="{5168B6C6-3075-49BB-9B41-7C670E6513CA}"/>
   </bookViews>
   <sheets>
     <sheet name="TwoxTwoScalar" sheetId="3" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="TwoxTwoCET-Scalar" sheetId="9" r:id="rId7"/>
     <sheet name="TwoxTwowOTax_IndCon" sheetId="10" r:id="rId8"/>
     <sheet name="TwoxTwoOutTax_1-2" sheetId="11" r:id="rId9"/>
+    <sheet name="TwoxTwo-ScalarOutNest" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="141">
   <si>
     <t>X.L</t>
   </si>
@@ -417,6 +418,45 @@
   </si>
   <si>
     <t>Itax=.1</t>
+  </si>
+  <si>
+    <t>FR.L</t>
+  </si>
+  <si>
+    <t>XU.L</t>
+  </si>
+  <si>
+    <t>PF.L</t>
+  </si>
+  <si>
+    <t>PXD.L</t>
+  </si>
+  <si>
+    <t>PXX.L</t>
+  </si>
+  <si>
+    <t>PKX.L</t>
+  </si>
+  <si>
+    <t>SYX.L</t>
+  </si>
+  <si>
+    <t>ROW.L</t>
+  </si>
+  <si>
+    <t>end=1.1</t>
+  </si>
+  <si>
+    <t>Itax=0.1</t>
+  </si>
+  <si>
+    <t>Otax=0.1</t>
+  </si>
+  <si>
+    <t>SXY.L</t>
+  </si>
+  <si>
+    <t>XP.L</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1197,711 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7EE3A2-0477-401B-9E37-E30271C46822}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.0087818924459078</v>
+      </c>
+      <c r="D2">
+        <v>1.0087818984480226</v>
+      </c>
+      <c r="E2">
+        <v>1.0087818924469572</v>
+      </c>
+      <c r="F2">
+        <v>0.80862897655434263</v>
+      </c>
+      <c r="G2">
+        <v>0.97382882042375429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0915655837604266</v>
+      </c>
+      <c r="D3">
+        <v>1.0915655804126048</v>
+      </c>
+      <c r="E3">
+        <v>1.0915655837428009</v>
+      </c>
+      <c r="F3">
+        <v>1.2594034491556683</v>
+      </c>
+      <c r="G3">
+        <v>1.121135937191029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.0503441611049424</v>
+      </c>
+      <c r="D4">
+        <v>1.0503441602079413</v>
+      </c>
+      <c r="E4">
+        <v>1.0503441610960742</v>
+      </c>
+      <c r="F4">
+        <v>1.0533658697164114</v>
+      </c>
+      <c r="G4">
+        <v>1.0514550815800936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.0363764562165405</v>
+      </c>
+      <c r="D5">
+        <v>1.0363764493185874</v>
+      </c>
+      <c r="E5">
+        <v>1.0363764562119133</v>
+      </c>
+      <c r="F5">
+        <v>0.958887134059208</v>
+      </c>
+      <c r="G5">
+        <v>1.022931192686233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.0363764562158884</v>
+      </c>
+      <c r="D7">
+        <v>1.0363764467002947</v>
+      </c>
+      <c r="E7">
+        <v>1.03637645621167</v>
+      </c>
+      <c r="F7">
+        <v>0.95888713402749703</v>
+      </c>
+      <c r="G7">
+        <v>1.0229311926913409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.017531272749113</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.0460796198843898</v>
+      </c>
+      <c r="F8">
+        <v>1.1303175404901751</v>
+      </c>
+      <c r="G8">
+        <v>1.1348010195250842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.98096444410281769</v>
+      </c>
+      <c r="D9">
+        <v>0.9640631895841022</v>
+      </c>
+      <c r="E9">
+        <v>1.0084868547104582</v>
+      </c>
+      <c r="F9">
+        <v>0.92696026052833602</v>
+      </c>
+      <c r="G9">
+        <v>1.063341999589474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.0039999207779782</v>
+      </c>
+      <c r="D10">
+        <v>0.98670178269616649</v>
+      </c>
+      <c r="E10">
+        <v>1.0321686257962945</v>
+      </c>
+      <c r="F10">
+        <v>1.0289368379244177</v>
+      </c>
+      <c r="G10">
+        <v>1.1040161208535313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.97270920241681125</v>
+      </c>
+      <c r="D11">
+        <v>0.95595017804950067</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1.0360238527648151</v>
+      </c>
+      <c r="D12">
+        <v>1.0181739667949257</v>
+      </c>
+      <c r="E12">
+        <v>1.0650910366187067</v>
+      </c>
+      <c r="F12">
+        <v>0.98436152085413908</v>
+      </c>
+      <c r="G12">
+        <v>1.050031164244674</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1.0545454545441773</v>
+      </c>
+      <c r="D13">
+        <v>1.0363764440814733</v>
+      </c>
+      <c r="E13">
+        <v>1.0841322893692942</v>
+      </c>
+      <c r="F13">
+        <v>1.083846947285189</v>
+      </c>
+      <c r="G13">
+        <v>1.1608233605436402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1.0175312727497825</v>
+      </c>
+      <c r="D14">
+        <v>1.0000000024997451</v>
+      </c>
+      <c r="E14">
+        <v>1.0460796198846283</v>
+      </c>
+      <c r="F14">
+        <v>1.1303175405730492</v>
+      </c>
+      <c r="G14">
+        <v>1.134801019517711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1.0175312727484433</v>
+      </c>
+      <c r="D15">
+        <v>0.99999999750029722</v>
+      </c>
+      <c r="E15">
+        <v>1.0460796198841524</v>
+      </c>
+      <c r="F15">
+        <v>1.1303175404116717</v>
+      </c>
+      <c r="G15">
+        <v>1.1348010195324607</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1.0545454545441773</v>
+      </c>
+      <c r="D16">
+        <v>1.0363764440814733</v>
+      </c>
+      <c r="E16">
+        <v>1.0841322893692942</v>
+      </c>
+      <c r="F16">
+        <v>1.083846947285189</v>
+      </c>
+      <c r="G16">
+        <v>1.1608233605436402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>80</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17">
+        <v>80</v>
+      </c>
+      <c r="G17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>80</v>
+      </c>
+      <c r="G19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+      <c r="G20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21">
+        <v>220</v>
+      </c>
+      <c r="C21">
+        <v>220</v>
+      </c>
+      <c r="D21">
+        <v>220</v>
+      </c>
+      <c r="E21">
+        <v>220</v>
+      </c>
+      <c r="F21">
+        <v>220</v>
+      </c>
+      <c r="G21">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>41.542442674765098</v>
+      </c>
+      <c r="D22">
+        <v>41.542442691088624</v>
+      </c>
+      <c r="E22">
+        <v>41.542442673943768</v>
+      </c>
+      <c r="F22">
+        <v>39.623493954449998</v>
+      </c>
+      <c r="G22">
+        <v>41.189005357666694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23">
+        <v>60</v>
+      </c>
+      <c r="C23">
+        <v>58.505481567020347</v>
+      </c>
+      <c r="D23">
+        <v>58.505481551694402</v>
+      </c>
+      <c r="E23">
+        <v>58.50548156779147</v>
+      </c>
+      <c r="F23">
+        <v>60.379484236749228</v>
+      </c>
+      <c r="G23">
+        <v>58.839689849532405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>80</v>
+      </c>
+      <c r="C24">
+        <v>82.535339520565458</v>
+      </c>
+      <c r="D24">
+        <v>82.535339547026339</v>
+      </c>
+      <c r="E24">
+        <v>82.5353395192341</v>
+      </c>
+      <c r="F24">
+        <v>79.370351203301908</v>
+      </c>
+      <c r="G24">
+        <v>81.960586873948159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>37.543075921873587</v>
+      </c>
+      <c r="D25">
+        <v>37.54307589702983</v>
+      </c>
+      <c r="E25">
+        <v>37.54307592312361</v>
+      </c>
+      <c r="F25">
+        <v>40.634635036712858</v>
+      </c>
+      <c r="G25">
+        <v>38.08656279327819</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26">
+        <v>80</v>
+      </c>
+      <c r="C26">
+        <v>78.936142616180291</v>
+      </c>
+      <c r="D26">
+        <v>78.936142557576616</v>
+      </c>
+      <c r="E26">
+        <v>78.936142616709958</v>
+      </c>
+      <c r="F26">
+        <v>72.82462143888138</v>
+      </c>
+      <c r="G26">
+        <v>77.829758828574981</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>102.34824787101159</v>
+      </c>
+      <c r="D27">
+        <v>102.34824777361034</v>
+      </c>
+      <c r="E27">
+        <v>102.34824786999235</v>
+      </c>
+      <c r="F27">
+        <v>111.00118108759018</v>
+      </c>
+      <c r="G27">
+        <v>103.82512129465007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28">
+        <v>220</v>
+      </c>
+      <c r="C28">
+        <v>231.07571544002587</v>
+      </c>
+      <c r="D28">
+        <v>231.07571525715505</v>
+      </c>
+      <c r="E28">
+        <v>231.07571544123067</v>
+      </c>
+      <c r="F28">
+        <v>231.74049138660823</v>
+      </c>
+      <c r="G28">
+        <v>231.32011801351359</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29">
+        <v>220</v>
+      </c>
+      <c r="C29">
+        <v>231.07571544002587</v>
+      </c>
+      <c r="D29">
+        <v>231.07571525715505</v>
+      </c>
+      <c r="E29">
+        <v>231.07571544123067</v>
+      </c>
+      <c r="F29">
+        <v>231.74049138660823</v>
+      </c>
+      <c r="G29">
+        <v>231.32011801351359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>220</v>
+      </c>
+      <c r="C30">
+        <v>232</v>
+      </c>
+      <c r="D30">
+        <v>228.00282018202665</v>
+      </c>
+      <c r="E30">
+        <v>238.50910366187065</v>
+      </c>
+      <c r="F30">
+        <v>238.44632842638742</v>
+      </c>
+      <c r="G30">
+        <v>255.38113936466033</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>21.090909090883546</v>
+      </c>
+      <c r="D31">
+        <v>20.727528881629468</v>
+      </c>
+      <c r="E31">
+        <v>21.682645787385884</v>
+      </c>
+      <c r="F31">
+        <v>21.676938945703782</v>
+      </c>
+      <c r="G31">
+        <v>23.216467210872803</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD2B994-3CF8-4777-9095-AA4EE6BD17EC}">
   <dimension ref="A1:F18"/>
@@ -3210,7 +3955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEAD0FC-6E99-420C-BC7A-3D842CD4A7CD}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>